<commit_message>
plus de valeurs test
</commit_message>
<xml_diff>
--- a/valeurs_expe.xlsx
+++ b/valeurs_expe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SU-ANNESOPHIE\Documents\GitHub\HEIG_ASD1_LABO_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B02B205-B65A-457C-8876-A10BE2784047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEAB056-2E11-4C6A-AF01-A4585BC57E47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{666A6892-ED96-4155-B69D-7B7D26C674DE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Fonction chercherPosition() :</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>Fct chercherSiContient() :</t>
+  </si>
+  <si>
+    <t>random2</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>(ancien)</t>
   </si>
 </sst>
 </file>
@@ -251,795 +260,6 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-CH"/>
-              <a:t>random</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>temps (ns)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.37069444444444444"/>
-                  <c:y val="0.2449537037037037"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="fr-FR"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Feuil1!$B$38:$B$41</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Feuil1!$C$38:$C$41</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>593200</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1988800</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>53808800</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>593628400</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-23CE-4819-8279-F4DEF5787601}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="465613712"/>
-        <c:axId val="465614040"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="465613712"/>
-        <c:scaling>
-          <c:logBase val="10"/>
-          <c:orientation val="minMax"/>
-          <c:min val="1000"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="465614040"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="465614040"/>
-        <c:scaling>
-          <c:logBase val="10"/>
-          <c:orientation val="minMax"/>
-          <c:min val="100000"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="465613712"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="fr-CH"/>
-              <a:t>random2</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.25194422572178476"/>
-                  <c:y val="0.19402777777777777"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="fr-FR"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Feuil1!$B$44:$B$48</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>729</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2187</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6561</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>19683</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>59049</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Feuil1!$C$44:$C$48</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>398400</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1220200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4703200</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80574200</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>683681800</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2D22-41AF-AC28-03631F079B79}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="624900856"/>
-        <c:axId val="624901512"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="624900856"/>
-        <c:scaling>
-          <c:logBase val="10"/>
-          <c:orientation val="minMax"/>
-          <c:min val="100"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="624901512"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="624901512"/>
-        <c:scaling>
-          <c:logBase val="10"/>
-          <c:orientation val="minMax"/>
-          <c:min val="100000"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="624900856"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="fr-CH"/>
               <a:t>fonction g</a:t>
             </a:r>
           </a:p>
@@ -1121,8 +341,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.36791666666666667"/>
-                  <c:y val="0.16102763196267134"/>
+                  <c:x val="-0.21292458725384672"/>
+                  <c:y val="0.1495434763117707"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1157,42 +377,54 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$B$32:$B$35</c:f>
+              <c:f>Feuil1!$B$34:$B$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10000</c:v>
+                  <c:v>6561</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100000</c:v>
+                  <c:v>19683</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000000</c:v>
+                  <c:v>59049</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000000</c:v>
+                  <c:v>177147</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>531441</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1594323</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$C$32:$C$35</c:f>
+              <c:f>Feuil1!$C$34:$C$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>140000</c:v>
+                  <c:v>85293</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1700000</c:v>
+                  <c:v>295245</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20000000</c:v>
+                  <c:v>944784</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>240000000</c:v>
+                  <c:v>3188646</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10628820</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33480783</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1284,7 +516,7 @@
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:min val="100000"/>
+          <c:min val="10000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1395,7 +627,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -1547,7 +779,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$B$22:$B$29</c:f>
+              <c:f>Feuil1!$B$24:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1580,7 +812,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$C$22:$C$29</c:f>
+              <c:f>Feuil1!$C$24:$C$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1808,7 +1040,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -1960,23 +1192,26 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$B$15:$B$19</c:f>
+              <c:f>Feuil1!$B$16:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
@@ -1984,23 +1219,26 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$C$15:$C$19</c:f>
+              <c:f>Feuil1!$C$16:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
@@ -2028,7 +1266,7 @@
         <c:axId val="465551192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="6"/>
+          <c:min val="5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2091,7 +1329,7 @@
         <c:axId val="465541352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="6"/>
+          <c:min val="5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2202,7 +1440,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -2354,23 +1592,26 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$B$8:$B$12</c:f>
+              <c:f>Feuil1!$B$8:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
@@ -2378,23 +1619,26 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$C$8:$C$12</c:f>
+              <c:f>Feuil1!$C$8:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>4032</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>16256</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>65280</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>261632</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1047552</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>4192256</c:v>
                 </c:pt>
               </c:numCache>
@@ -2486,7 +1730,7 @@
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:min val="10000"/>
+          <c:min val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2597,7 +1841,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -2699,7 +1943,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$A$52:$A$61</c:f>
+              <c:f>Feuil1!$A$56:$A$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2738,7 +1982,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$B$52:$B$61</c:f>
+              <c:f>Feuil1!$B$56:$B$65</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2918,6 +2162,785 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="465625192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CH"/>
+              <a:t>random2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.5356517935258092E-2"/>
+                  <c:y val="8.6468358121901431E-4"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$A$69:$A$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>105000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$B$69:$B$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6256000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46871800</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>181206600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>480430600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1077662400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2179729600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D2C5-4294-901F-95EC4F38BE9E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="537466896"/>
+        <c:axId val="537467224"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="537466896"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="1000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="537467224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="537467224"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="1000000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="537466896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.21887685914260718"/>
+                  <c:y val="-5.0123942840478277E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$A$77:$A$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>177147</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>531441</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1594323</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4782969</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14348907</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43046721</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$B$77:$B$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9609000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31241400</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96852200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>284821800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>809747800</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2433408400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7512-426F-A23A-3C04FF5125CC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="585581824"/>
+        <c:axId val="585582480"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="585581824"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="100000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="585582480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="585582480"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="1000000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="585581824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6869,23 +6892,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>178593</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>130969</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>180782</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>85115</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>178593</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>154781</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>180780</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>117140</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Graphique 1">
+        <xdr:cNvPr id="4" name="Graphique 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8548E513-3E3E-4C5D-BFAD-EE716AF3F847}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CAC2C60-EDCE-455D-95BA-932BC81798F1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6905,23 +6928,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>640556</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>50007</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>705068</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>24815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>640556</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>73819</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>705070</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>53062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Graphique 2">
+        <xdr:cNvPr id="5" name="Graphique 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E5B2A82-B838-404A-BC0F-AF4171040A60}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F73D33B-F625-4431-8EBA-AF40AB1F9678}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6941,23 +6964,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>154780</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>7144</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>448649</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>53641</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>154780</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>30956</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>448647</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>82215</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Graphique 3">
+        <xdr:cNvPr id="6" name="Graphique 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CAC2C60-EDCE-455D-95BA-932BC81798F1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2F5A495-7280-47A8-9BE9-80915A508F29}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6977,23 +7000,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>230980</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>169068</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>411165</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>131226</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>230980</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>16668</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>411167</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>159802</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Graphique 4">
+        <xdr:cNvPr id="7" name="Graphique 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F73D33B-F625-4431-8EBA-AF40AB1F9678}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBFB8CBE-2BEC-47BA-8AB8-24E8F3F7DCD2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7013,23 +7036,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>150018</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>97631</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>105104</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>161018</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>150018</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>126206</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>105105</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>17229</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Graphique 5">
+        <xdr:cNvPr id="10" name="Graphique 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2F5A495-7280-47A8-9BE9-80915A508F29}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B91EDD04-7D97-4E8E-AE84-84DEDBC21A2E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7049,23 +7072,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>35719</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>69056</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>282800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>64079</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>35719</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>97631</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>282801</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>117867</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Graphique 6">
+        <xdr:cNvPr id="8" name="Graphique 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBFB8CBE-2BEC-47BA-8AB8-24E8F3F7DCD2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDC30D74-453F-43ED-B095-6E5C365F4078}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7085,23 +7108,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>283367</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>111918</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>274246</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>129693</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>283367</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>140493</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>274247</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>183481</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Graphique 9">
+        <xdr:cNvPr id="9" name="Graphique 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B91EDD04-7D97-4E8E-AE84-84DEDBC21A2E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1587AE62-E763-4FF5-B8EA-77E3B1C1943C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7419,10 +7442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85499602-D119-4872-92A1-2FAD642673CF}">
-  <dimension ref="A1:T61"/>
+  <dimension ref="A1:T82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="48" workbookViewId="0">
+      <selection activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7562,1115 +7585,1457 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B8" s="3">
-        <v>7</v>
-      </c>
-      <c r="C8" s="4">
-        <v>16256</v>
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>4032</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B9" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="4">
-        <v>65280</v>
+        <v>16256</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B10" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="4">
-        <v>261632</v>
+        <v>65280</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B11" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="4">
-        <v>1047552</v>
+        <v>261632</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B12" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="4">
-        <v>4192256</v>
+        <v>1047552</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B13" s="3"/>
-      <c r="C13" s="4"/>
+      <c r="B13" s="3">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4">
+        <v>4192256</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B15" s="3">
-        <v>7</v>
-      </c>
-      <c r="C15" s="4">
-        <v>7</v>
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B16" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C16" s="4">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B17" s="3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C17" s="4">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B18" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C18" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B19" s="3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C19" s="4">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B20" s="3"/>
-      <c r="C20" s="4"/>
+      <c r="B20" s="3">
+        <v>10</v>
+      </c>
+      <c r="C20" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>18</v>
+      <c r="B21" s="3">
+        <v>11</v>
+      </c>
+      <c r="C21" s="4">
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B22" s="3">
-        <v>11</v>
-      </c>
-      <c r="C22" s="4">
-        <v>177147</v>
-      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B23" s="3">
-        <v>12</v>
-      </c>
-      <c r="C23" s="4">
-        <v>531441</v>
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B24" s="3">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C24" s="4">
-        <v>1594323</v>
+        <v>177147</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B25" s="3">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C25" s="4">
-        <v>4782969</v>
+        <v>531441</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B26" s="3">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C26" s="4">
-        <v>14348907</v>
+        <v>1594323</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B27" s="3">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C27" s="4">
-        <v>43046721</v>
+        <v>4782969</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B28" s="3">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C28" s="4">
-        <v>129140163</v>
+        <v>14348907</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B29" s="3">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C29" s="4">
-        <v>387420489</v>
+        <v>43046721</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B30" s="3"/>
-      <c r="C30" s="4"/>
+      <c r="B30" s="3">
+        <v>17</v>
+      </c>
+      <c r="C30" s="4">
+        <v>129140163</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>17</v>
+      <c r="B31" s="3">
+        <v>18</v>
+      </c>
+      <c r="C31" s="4">
+        <v>387420489</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B32" s="3">
-        <v>10000</v>
-      </c>
-      <c r="C32" s="4">
-        <v>140000</v>
-      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="4"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B33" s="3">
-        <v>100000</v>
-      </c>
-      <c r="C33" s="4">
-        <v>1700000</v>
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B34" s="3">
-        <v>1000000</v>
-      </c>
-      <c r="C34" s="4">
-        <v>20000000</v>
+      <c r="B34">
+        <v>6561</v>
+      </c>
+      <c r="C34">
+        <v>85293</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B35" s="3">
-        <v>10000000</v>
-      </c>
-      <c r="C35" s="4">
-        <v>240000000</v>
+      <c r="B35">
+        <v>19683</v>
+      </c>
+      <c r="C35">
+        <v>295245</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B36" s="3"/>
-      <c r="C36" s="4"/>
+      <c r="B36">
+        <v>59049</v>
+      </c>
+      <c r="C36">
+        <v>944784</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>16</v>
+      <c r="B37">
+        <v>177147</v>
+      </c>
+      <c r="C37">
+        <v>3188646</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B38" s="3">
-        <v>10000</v>
-      </c>
-      <c r="C38" s="4">
-        <f>AVERAGE(D38:H38)</f>
-        <v>593200</v>
-      </c>
-      <c r="D38">
-        <v>985000</v>
-      </c>
-      <c r="E38">
-        <v>997000</v>
-      </c>
-      <c r="F38">
-        <v>984000</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
+      <c r="B38">
+        <v>531441</v>
+      </c>
+      <c r="C38">
+        <v>10628820</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B39" s="3">
-        <v>100000</v>
-      </c>
-      <c r="C39" s="4">
-        <f>AVERAGE(D39:H39)</f>
-        <v>1988800</v>
-      </c>
-      <c r="D39">
-        <v>997000</v>
-      </c>
-      <c r="E39">
-        <v>3974000</v>
-      </c>
-      <c r="F39">
-        <v>986000</v>
-      </c>
-      <c r="G39">
-        <v>998000</v>
-      </c>
-      <c r="H39">
-        <v>2989000</v>
+      <c r="B39">
+        <v>1594323</v>
+      </c>
+      <c r="C39">
+        <v>33480783</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B40" s="3">
-        <v>1000000</v>
-      </c>
-      <c r="C40" s="4">
-        <f>AVERAGE(D40:H40)</f>
-        <v>53808800</v>
-      </c>
-      <c r="D40">
-        <v>55319000</v>
-      </c>
-      <c r="E40">
-        <v>48248000</v>
-      </c>
-      <c r="F40">
-        <v>60853000</v>
-      </c>
-      <c r="G40">
-        <v>58681000</v>
-      </c>
-      <c r="H40">
-        <v>45943000</v>
-      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="4"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B41" s="3">
-        <v>10000000</v>
-      </c>
-      <c r="C41" s="4">
-        <f>AVERAGE(D41:H41)</f>
-        <v>593628400</v>
-      </c>
-      <c r="D41">
-        <v>605512000</v>
-      </c>
-      <c r="E41">
-        <v>581709000</v>
-      </c>
-      <c r="F41">
-        <v>603540000</v>
-      </c>
-      <c r="G41">
-        <v>595658000</v>
-      </c>
-      <c r="H41">
-        <v>581723000</v>
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B42" s="3"/>
-      <c r="C42" s="4"/>
+      <c r="A42" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C42" s="4">
+        <f>AVERAGE(D42:H42)</f>
+        <v>593200</v>
+      </c>
+      <c r="D42">
+        <v>985000</v>
+      </c>
+      <c r="E42">
+        <v>997000</v>
+      </c>
+      <c r="F42">
+        <v>984000</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>5</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>16</v>
+      <c r="B43" s="3">
+        <v>100000</v>
+      </c>
+      <c r="C43" s="4">
+        <f>AVERAGE(D43:H43)</f>
+        <v>1988800</v>
+      </c>
+      <c r="D43">
+        <v>997000</v>
+      </c>
+      <c r="E43">
+        <v>3974000</v>
+      </c>
+      <c r="F43">
+        <v>986000</v>
+      </c>
+      <c r="G43">
+        <v>998000</v>
+      </c>
+      <c r="H43">
+        <v>2989000</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B44" s="3">
-        <v>729</v>
+        <v>1000000</v>
       </c>
       <c r="C44" s="4">
         <f>AVERAGE(D44:H44)</f>
-        <v>398400</v>
+        <v>53808800</v>
       </c>
       <c r="D44">
-        <v>997000</v>
+        <v>55319000</v>
       </c>
       <c r="E44">
-        <v>995000</v>
+        <v>48248000</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>60853000</v>
       </c>
       <c r="G44">
-        <v>0</v>
+        <v>58681000</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>45943000</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B45" s="3">
-        <v>2187</v>
+        <v>10000000</v>
       </c>
       <c r="C45" s="4">
         <f>AVERAGE(D45:H45)</f>
-        <v>1220200</v>
+        <v>593628400</v>
       </c>
       <c r="D45">
-        <v>999000</v>
+        <v>605512000</v>
       </c>
       <c r="E45">
-        <v>999000</v>
+        <v>581709000</v>
       </c>
       <c r="F45">
-        <v>1000000</v>
+        <v>603540000</v>
       </c>
       <c r="G45">
-        <v>984000</v>
+        <v>595658000</v>
       </c>
       <c r="H45">
-        <v>2119000</v>
+        <v>581723000</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B46" s="3">
-        <v>6561</v>
-      </c>
-      <c r="C46" s="4">
-        <f>AVERAGE(D46:H46)</f>
-        <v>4703200</v>
-      </c>
-      <c r="D46">
-        <v>1024000</v>
-      </c>
-      <c r="E46">
-        <v>4435000</v>
-      </c>
-      <c r="F46">
-        <v>994000</v>
-      </c>
-      <c r="G46">
-        <v>10459000</v>
-      </c>
-      <c r="H46">
-        <v>6604000</v>
-      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="4"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B47" s="3">
-        <v>19683</v>
-      </c>
-      <c r="C47" s="4">
-        <f>AVERAGE(D47:H47)</f>
-        <v>80574200</v>
-      </c>
-      <c r="D47">
-        <v>81107000</v>
-      </c>
-      <c r="E47">
-        <v>83683000</v>
-      </c>
-      <c r="F47">
-        <v>82610000</v>
-      </c>
-      <c r="G47">
-        <v>80129000</v>
-      </c>
-      <c r="H47">
-        <v>75342000</v>
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B48" s="5">
-        <v>59049</v>
-      </c>
-      <c r="C48" s="6">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="3">
+        <v>729</v>
+      </c>
+      <c r="C48" s="4">
         <f>AVERAGE(D48:H48)</f>
-        <v>683681800</v>
+        <v>398400</v>
       </c>
       <c r="D48">
-        <v>685048000</v>
+        <v>997000</v>
       </c>
       <c r="E48">
-        <v>694360000</v>
+        <v>995000</v>
       </c>
       <c r="F48">
-        <v>683357000</v>
+        <v>0</v>
       </c>
       <c r="G48">
-        <v>671998000</v>
+        <v>0</v>
       </c>
       <c r="H48">
-        <v>683646000</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="B49" s="3">
+        <v>2187</v>
+      </c>
+      <c r="C49" s="4">
+        <f>AVERAGE(D49:H49)</f>
+        <v>1220200</v>
+      </c>
+      <c r="D49">
+        <v>999000</v>
+      </c>
+      <c r="E49">
+        <v>999000</v>
+      </c>
+      <c r="F49">
+        <v>1000000</v>
+      </c>
+      <c r="G49">
+        <v>984000</v>
+      </c>
+      <c r="H49">
+        <v>2119000</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
-        <v>0</v>
+      <c r="B50" s="3">
+        <v>6561</v>
+      </c>
+      <c r="C50" s="4">
+        <f>AVERAGE(D50:H50)</f>
+        <v>4703200</v>
+      </c>
+      <c r="D50">
+        <v>1024000</v>
+      </c>
+      <c r="E50">
+        <v>4435000</v>
+      </c>
+      <c r="F50">
+        <v>994000</v>
+      </c>
+      <c r="G50">
+        <v>10459000</v>
+      </c>
+      <c r="H50">
+        <v>6604000</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
-        <v>13</v>
-      </c>
-      <c r="B51" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" t="s">
-        <v>14</v>
+      <c r="B51" s="3">
+        <v>19683</v>
+      </c>
+      <c r="C51" s="4">
+        <f>AVERAGE(D51:H51)</f>
+        <v>80574200</v>
+      </c>
+      <c r="D51">
+        <v>81107000</v>
+      </c>
+      <c r="E51">
+        <v>83683000</v>
+      </c>
+      <c r="F51">
+        <v>82610000</v>
+      </c>
+      <c r="G51">
+        <v>80129000</v>
+      </c>
+      <c r="H51">
+        <v>75342000</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A52">
-        <v>2187</v>
-      </c>
-      <c r="B52" s="7">
-        <f>AVERAGE(C52:T52)</f>
-        <v>1260.4444444444443</v>
-      </c>
-      <c r="C52">
-        <v>366</v>
+    <row r="52" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B52" s="5">
+        <v>59049</v>
+      </c>
+      <c r="C52" s="6">
+        <f>AVERAGE(D52:H52)</f>
+        <v>683681800</v>
       </c>
       <c r="D52">
-        <v>2187</v>
+        <v>685048000</v>
       </c>
       <c r="E52">
-        <v>2187</v>
+        <v>694360000</v>
       </c>
       <c r="F52">
-        <v>375</v>
+        <v>683357000</v>
       </c>
       <c r="G52">
-        <v>1349</v>
+        <v>671998000</v>
       </c>
       <c r="H52">
-        <v>1569</v>
-      </c>
-      <c r="I52">
-        <v>292</v>
-      </c>
-      <c r="J52">
-        <v>29</v>
-      </c>
-      <c r="K52">
-        <v>2187</v>
-      </c>
-      <c r="L52">
-        <v>945</v>
-      </c>
-      <c r="M52">
-        <v>1</v>
-      </c>
-      <c r="N52">
-        <v>2187</v>
-      </c>
-      <c r="O52">
-        <v>719</v>
-      </c>
-      <c r="P52">
-        <v>2187</v>
-      </c>
-      <c r="Q52">
-        <v>873</v>
-      </c>
-      <c r="R52">
-        <v>2187</v>
-      </c>
-      <c r="S52">
-        <v>861</v>
-      </c>
-      <c r="T52">
-        <v>2187</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A53">
-        <v>6561</v>
-      </c>
-      <c r="B53" s="7">
-        <f t="shared" ref="B53:B61" si="0">AVERAGE(C53:T53)</f>
-        <v>3730.0555555555557</v>
-      </c>
-      <c r="C53">
-        <v>6561</v>
-      </c>
-      <c r="D53">
-        <v>1911</v>
-      </c>
-      <c r="E53">
-        <v>6561</v>
-      </c>
-      <c r="F53">
-        <v>6561</v>
-      </c>
-      <c r="G53">
-        <v>2830</v>
-      </c>
-      <c r="H53">
-        <v>6561</v>
-      </c>
-      <c r="I53">
-        <v>251</v>
-      </c>
-      <c r="J53">
-        <v>1862</v>
-      </c>
-      <c r="K53">
-        <v>1121</v>
-      </c>
-      <c r="L53">
-        <v>6561</v>
-      </c>
-      <c r="M53">
-        <v>1873</v>
-      </c>
-      <c r="N53">
-        <v>6561</v>
-      </c>
-      <c r="O53">
-        <v>2450</v>
-      </c>
-      <c r="P53">
-        <v>5912</v>
-      </c>
-      <c r="Q53">
-        <v>1781</v>
-      </c>
-      <c r="R53">
-        <v>2447</v>
-      </c>
-      <c r="S53">
-        <v>4515</v>
-      </c>
-      <c r="T53">
-        <v>822</v>
+        <v>683646000</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A54">
-        <v>19683</v>
-      </c>
-      <c r="B54" s="7">
-        <f t="shared" si="0"/>
-        <v>11317.666666666666</v>
-      </c>
-      <c r="C54">
-        <v>19683</v>
-      </c>
-      <c r="D54">
-        <v>19683</v>
-      </c>
-      <c r="E54">
-        <v>10621</v>
-      </c>
-      <c r="F54">
-        <v>5780</v>
-      </c>
-      <c r="G54">
-        <v>13198</v>
-      </c>
-      <c r="H54">
-        <v>5538</v>
-      </c>
-      <c r="I54">
-        <v>3120</v>
-      </c>
-      <c r="J54">
-        <v>3856</v>
-      </c>
-      <c r="K54">
-        <v>15785</v>
-      </c>
-      <c r="L54">
-        <v>5835</v>
-      </c>
-      <c r="M54">
-        <v>19683</v>
-      </c>
-      <c r="N54">
-        <v>19683</v>
-      </c>
-      <c r="O54">
-        <v>9693</v>
-      </c>
-      <c r="P54">
-        <v>2598</v>
-      </c>
-      <c r="Q54">
-        <v>8315</v>
-      </c>
-      <c r="R54">
-        <v>4577</v>
-      </c>
-      <c r="S54">
-        <v>19683</v>
-      </c>
-      <c r="T54">
-        <v>16387</v>
+      <c r="A54" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A55">
-        <v>59049</v>
-      </c>
-      <c r="B55" s="7">
-        <f t="shared" si="0"/>
-        <v>19679.111111111109</v>
-      </c>
-      <c r="C55">
-        <v>31689</v>
-      </c>
-      <c r="D55">
-        <v>35967</v>
-      </c>
-      <c r="E55">
-        <v>9640</v>
-      </c>
-      <c r="F55">
-        <v>20815</v>
-      </c>
-      <c r="G55">
-        <v>59049</v>
-      </c>
-      <c r="H55">
-        <v>8335</v>
-      </c>
-      <c r="I55">
-        <v>3574</v>
-      </c>
-      <c r="J55">
-        <v>19763</v>
-      </c>
-      <c r="K55">
-        <v>8736</v>
-      </c>
-      <c r="L55">
-        <v>12932</v>
-      </c>
-      <c r="M55">
-        <v>21102</v>
-      </c>
-      <c r="N55">
-        <v>5384</v>
-      </c>
-      <c r="O55">
-        <v>15616</v>
-      </c>
-      <c r="P55">
-        <v>7312</v>
-      </c>
-      <c r="Q55">
-        <v>6214</v>
-      </c>
-      <c r="R55">
-        <v>6131</v>
-      </c>
-      <c r="S55">
-        <v>30699</v>
-      </c>
-      <c r="T55">
-        <v>51266</v>
+      <c r="A55" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A56">
-        <v>177147</v>
+        <v>2187</v>
       </c>
       <c r="B56" s="7">
-        <f t="shared" si="0"/>
-        <v>36239</v>
+        <f>AVERAGE(C56:T56)</f>
+        <v>1260.4444444444443</v>
       </c>
       <c r="C56">
-        <v>6046</v>
+        <v>366</v>
       </c>
       <c r="D56">
-        <v>9002</v>
+        <v>2187</v>
       </c>
       <c r="E56">
-        <v>1048</v>
+        <v>2187</v>
       </c>
       <c r="F56">
-        <v>1479</v>
+        <v>375</v>
       </c>
       <c r="G56">
-        <v>128550</v>
+        <v>1349</v>
       </c>
       <c r="H56">
-        <v>65341</v>
+        <v>1569</v>
       </c>
       <c r="I56">
-        <v>86493</v>
+        <v>292</v>
       </c>
       <c r="J56">
-        <v>51118</v>
+        <v>29</v>
       </c>
       <c r="K56">
-        <v>88916</v>
+        <v>2187</v>
       </c>
       <c r="L56">
-        <v>38019</v>
+        <v>945</v>
       </c>
       <c r="M56">
-        <v>2597</v>
+        <v>1</v>
       </c>
       <c r="N56">
-        <v>17427</v>
+        <v>2187</v>
       </c>
       <c r="O56">
-        <v>23990</v>
+        <v>719</v>
       </c>
       <c r="P56">
-        <v>7196</v>
+        <v>2187</v>
       </c>
       <c r="Q56">
-        <v>13133</v>
+        <v>873</v>
       </c>
       <c r="R56">
-        <v>3588</v>
+        <v>2187</v>
       </c>
       <c r="S56">
-        <v>68198</v>
+        <v>861</v>
       </c>
       <c r="T56">
-        <v>40161</v>
+        <v>2187</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A57">
-        <v>531441</v>
+        <v>6561</v>
       </c>
       <c r="B57" s="7">
-        <f t="shared" si="0"/>
-        <v>45113.5</v>
+        <f t="shared" ref="B57:B65" si="0">AVERAGE(C57:T57)</f>
+        <v>3730.0555555555557</v>
       </c>
       <c r="C57">
-        <v>133180</v>
+        <v>6561</v>
       </c>
       <c r="D57">
-        <v>26235</v>
+        <v>1911</v>
       </c>
       <c r="E57">
-        <v>60413</v>
+        <v>6561</v>
       </c>
       <c r="F57">
-        <v>3575</v>
+        <v>6561</v>
       </c>
       <c r="G57">
-        <v>3253</v>
+        <v>2830</v>
       </c>
       <c r="H57">
-        <v>8815</v>
+        <v>6561</v>
       </c>
       <c r="I57">
-        <v>32539</v>
+        <v>251</v>
       </c>
       <c r="J57">
-        <v>33490</v>
+        <v>1862</v>
       </c>
       <c r="K57">
-        <v>41342</v>
+        <v>1121</v>
       </c>
       <c r="L57">
-        <v>85069</v>
+        <v>6561</v>
       </c>
       <c r="M57">
-        <v>18189</v>
+        <v>1873</v>
       </c>
       <c r="N57">
-        <v>11061</v>
+        <v>6561</v>
       </c>
       <c r="O57">
-        <v>30361</v>
+        <v>2450</v>
       </c>
       <c r="P57">
-        <v>65486</v>
+        <v>5912</v>
       </c>
       <c r="Q57">
-        <v>14043</v>
+        <v>1781</v>
       </c>
       <c r="R57">
-        <v>105883</v>
+        <v>2447</v>
       </c>
       <c r="S57">
-        <v>116308</v>
+        <v>4515</v>
       </c>
       <c r="T57">
-        <v>22801</v>
+        <v>822</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A58">
-        <v>1594323</v>
+        <v>19683</v>
       </c>
       <c r="B58" s="7">
         <f t="shared" si="0"/>
-        <v>27865.055555555555</v>
+        <v>11317.666666666666</v>
       </c>
       <c r="C58">
-        <v>8984</v>
+        <v>19683</v>
       </c>
       <c r="D58">
-        <v>6852</v>
+        <v>19683</v>
       </c>
       <c r="E58">
-        <v>20653</v>
+        <v>10621</v>
       </c>
       <c r="F58">
-        <v>13347</v>
+        <v>5780</v>
       </c>
       <c r="G58">
-        <v>22039</v>
+        <v>13198</v>
       </c>
       <c r="H58">
-        <v>31754</v>
+        <v>5538</v>
       </c>
       <c r="I58">
-        <v>26706</v>
+        <v>3120</v>
       </c>
       <c r="J58">
-        <v>28490</v>
+        <v>3856</v>
       </c>
       <c r="K58">
-        <v>7932</v>
+        <v>15785</v>
       </c>
       <c r="L58">
-        <v>3432</v>
+        <v>5835</v>
       </c>
       <c r="M58">
-        <v>54081</v>
+        <v>19683</v>
       </c>
       <c r="N58">
-        <v>1456</v>
+        <v>19683</v>
       </c>
       <c r="O58">
-        <v>67632</v>
+        <v>9693</v>
       </c>
       <c r="P58">
-        <v>32474</v>
+        <v>2598</v>
       </c>
       <c r="Q58">
-        <v>27816</v>
+        <v>8315</v>
       </c>
       <c r="R58">
-        <v>10809</v>
+        <v>4577</v>
       </c>
       <c r="S58">
-        <v>32309</v>
+        <v>19683</v>
       </c>
       <c r="T58">
-        <v>104805</v>
+        <v>16387</v>
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A59">
-        <v>4782969</v>
+        <v>59049</v>
       </c>
       <c r="B59" s="7">
         <f t="shared" si="0"/>
-        <v>25362.666666666668</v>
+        <v>19679.111111111109</v>
       </c>
       <c r="C59">
-        <v>14127</v>
+        <v>31689</v>
       </c>
       <c r="D59">
-        <v>23135</v>
+        <v>35967</v>
       </c>
       <c r="E59">
-        <v>44608</v>
+        <v>9640</v>
       </c>
       <c r="F59">
-        <v>20990</v>
+        <v>20815</v>
       </c>
       <c r="G59">
-        <v>1577</v>
+        <v>59049</v>
       </c>
       <c r="H59">
-        <v>31020</v>
+        <v>8335</v>
       </c>
       <c r="I59">
-        <v>8519</v>
+        <v>3574</v>
       </c>
       <c r="J59">
-        <v>4766</v>
+        <v>19763</v>
       </c>
       <c r="K59">
-        <v>11822</v>
+        <v>8736</v>
       </c>
       <c r="L59">
-        <v>129465</v>
+        <v>12932</v>
       </c>
       <c r="M59">
-        <v>2809</v>
+        <v>21102</v>
       </c>
       <c r="N59">
-        <v>10758</v>
+        <v>5384</v>
       </c>
       <c r="O59">
-        <v>6560</v>
+        <v>15616</v>
       </c>
       <c r="P59">
-        <v>28158</v>
+        <v>7312</v>
       </c>
       <c r="Q59">
-        <v>53995</v>
+        <v>6214</v>
       </c>
       <c r="R59">
-        <v>19104</v>
+        <v>6131</v>
       </c>
       <c r="S59">
-        <v>19469</v>
+        <v>30699</v>
       </c>
       <c r="T59">
-        <v>25646</v>
+        <v>51266</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A60">
-        <v>14348907</v>
+        <v>177147</v>
       </c>
       <c r="B60" s="7">
         <f t="shared" si="0"/>
-        <v>48379.166666666664</v>
+        <v>36239</v>
       </c>
       <c r="C60">
-        <v>73678</v>
+        <v>6046</v>
       </c>
       <c r="D60">
-        <v>84372</v>
+        <v>9002</v>
       </c>
       <c r="E60">
-        <v>9553</v>
+        <v>1048</v>
       </c>
       <c r="F60">
-        <v>29145</v>
+        <v>1479</v>
       </c>
       <c r="G60">
-        <v>110454</v>
+        <v>128550</v>
       </c>
       <c r="H60">
-        <v>178094</v>
+        <v>65341</v>
       </c>
       <c r="I60">
-        <v>27430</v>
+        <v>86493</v>
       </c>
       <c r="J60">
-        <v>40054</v>
+        <v>51118</v>
       </c>
       <c r="K60">
-        <v>85025</v>
+        <v>88916</v>
       </c>
       <c r="L60">
-        <v>45779</v>
+        <v>38019</v>
       </c>
       <c r="M60">
-        <v>25978</v>
+        <v>2597</v>
       </c>
       <c r="N60">
-        <v>6729</v>
+        <v>17427</v>
       </c>
       <c r="O60">
-        <v>39747</v>
+        <v>23990</v>
       </c>
       <c r="P60">
-        <v>2270</v>
+        <v>7196</v>
       </c>
       <c r="Q60">
-        <v>48145</v>
+        <v>13133</v>
       </c>
       <c r="R60">
-        <v>28270</v>
+        <v>3588</v>
       </c>
       <c r="S60">
-        <v>5169</v>
+        <v>68198</v>
       </c>
       <c r="T60">
-        <v>30933</v>
+        <v>40161</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A61">
-        <v>43046721</v>
+        <v>531441</v>
       </c>
       <c r="B61" s="7">
         <f t="shared" si="0"/>
+        <v>45113.5</v>
+      </c>
+      <c r="C61">
+        <v>133180</v>
+      </c>
+      <c r="D61">
+        <v>26235</v>
+      </c>
+      <c r="E61">
+        <v>60413</v>
+      </c>
+      <c r="F61">
+        <v>3575</v>
+      </c>
+      <c r="G61">
+        <v>3253</v>
+      </c>
+      <c r="H61">
+        <v>8815</v>
+      </c>
+      <c r="I61">
+        <v>32539</v>
+      </c>
+      <c r="J61">
+        <v>33490</v>
+      </c>
+      <c r="K61">
+        <v>41342</v>
+      </c>
+      <c r="L61">
+        <v>85069</v>
+      </c>
+      <c r="M61">
+        <v>18189</v>
+      </c>
+      <c r="N61">
+        <v>11061</v>
+      </c>
+      <c r="O61">
+        <v>30361</v>
+      </c>
+      <c r="P61">
+        <v>65486</v>
+      </c>
+      <c r="Q61">
+        <v>14043</v>
+      </c>
+      <c r="R61">
+        <v>105883</v>
+      </c>
+      <c r="S61">
+        <v>116308</v>
+      </c>
+      <c r="T61">
+        <v>22801</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>1594323</v>
+      </c>
+      <c r="B62" s="7">
+        <f t="shared" si="0"/>
+        <v>27865.055555555555</v>
+      </c>
+      <c r="C62">
+        <v>8984</v>
+      </c>
+      <c r="D62">
+        <v>6852</v>
+      </c>
+      <c r="E62">
+        <v>20653</v>
+      </c>
+      <c r="F62">
+        <v>13347</v>
+      </c>
+      <c r="G62">
+        <v>22039</v>
+      </c>
+      <c r="H62">
+        <v>31754</v>
+      </c>
+      <c r="I62">
+        <v>26706</v>
+      </c>
+      <c r="J62">
+        <v>28490</v>
+      </c>
+      <c r="K62">
+        <v>7932</v>
+      </c>
+      <c r="L62">
+        <v>3432</v>
+      </c>
+      <c r="M62">
+        <v>54081</v>
+      </c>
+      <c r="N62">
+        <v>1456</v>
+      </c>
+      <c r="O62">
+        <v>67632</v>
+      </c>
+      <c r="P62">
+        <v>32474</v>
+      </c>
+      <c r="Q62">
+        <v>27816</v>
+      </c>
+      <c r="R62">
+        <v>10809</v>
+      </c>
+      <c r="S62">
+        <v>32309</v>
+      </c>
+      <c r="T62">
+        <v>104805</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>4782969</v>
+      </c>
+      <c r="B63" s="7">
+        <f t="shared" si="0"/>
+        <v>25362.666666666668</v>
+      </c>
+      <c r="C63">
+        <v>14127</v>
+      </c>
+      <c r="D63">
+        <v>23135</v>
+      </c>
+      <c r="E63">
+        <v>44608</v>
+      </c>
+      <c r="F63">
+        <v>20990</v>
+      </c>
+      <c r="G63">
+        <v>1577</v>
+      </c>
+      <c r="H63">
+        <v>31020</v>
+      </c>
+      <c r="I63">
+        <v>8519</v>
+      </c>
+      <c r="J63">
+        <v>4766</v>
+      </c>
+      <c r="K63">
+        <v>11822</v>
+      </c>
+      <c r="L63">
+        <v>129465</v>
+      </c>
+      <c r="M63">
+        <v>2809</v>
+      </c>
+      <c r="N63">
+        <v>10758</v>
+      </c>
+      <c r="O63">
+        <v>6560</v>
+      </c>
+      <c r="P63">
+        <v>28158</v>
+      </c>
+      <c r="Q63">
+        <v>53995</v>
+      </c>
+      <c r="R63">
+        <v>19104</v>
+      </c>
+      <c r="S63">
+        <v>19469</v>
+      </c>
+      <c r="T63">
+        <v>25646</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>14348907</v>
+      </c>
+      <c r="B64" s="7">
+        <f t="shared" si="0"/>
+        <v>48379.166666666664</v>
+      </c>
+      <c r="C64">
+        <v>73678</v>
+      </c>
+      <c r="D64">
+        <v>84372</v>
+      </c>
+      <c r="E64">
+        <v>9553</v>
+      </c>
+      <c r="F64">
+        <v>29145</v>
+      </c>
+      <c r="G64">
+        <v>110454</v>
+      </c>
+      <c r="H64">
+        <v>178094</v>
+      </c>
+      <c r="I64">
+        <v>27430</v>
+      </c>
+      <c r="J64">
+        <v>40054</v>
+      </c>
+      <c r="K64">
+        <v>85025</v>
+      </c>
+      <c r="L64">
+        <v>45779</v>
+      </c>
+      <c r="M64">
+        <v>25978</v>
+      </c>
+      <c r="N64">
+        <v>6729</v>
+      </c>
+      <c r="O64">
+        <v>39747</v>
+      </c>
+      <c r="P64">
+        <v>2270</v>
+      </c>
+      <c r="Q64">
+        <v>48145</v>
+      </c>
+      <c r="R64">
+        <v>28270</v>
+      </c>
+      <c r="S64">
+        <v>5169</v>
+      </c>
+      <c r="T64">
+        <v>30933</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>43046721</v>
+      </c>
+      <c r="B65" s="7">
+        <f t="shared" si="0"/>
         <v>25881.777777777777</v>
       </c>
-      <c r="C61">
+      <c r="C65">
         <v>46247</v>
       </c>
-      <c r="D61">
+      <c r="D65">
         <v>615</v>
       </c>
-      <c r="E61">
+      <c r="E65">
         <v>26296</v>
       </c>
-      <c r="F61">
+      <c r="F65">
         <v>62149</v>
       </c>
-      <c r="G61">
+      <c r="G65">
         <v>58821</v>
       </c>
-      <c r="H61">
+      <c r="H65">
         <v>34933</v>
       </c>
-      <c r="I61">
+      <c r="I65">
         <v>25047</v>
       </c>
-      <c r="J61">
+      <c r="J65">
         <v>25519</v>
       </c>
-      <c r="K61">
+      <c r="K65">
         <v>7956</v>
       </c>
-      <c r="L61">
+      <c r="L65">
         <v>5543</v>
       </c>
-      <c r="M61">
+      <c r="M65">
         <v>35622</v>
       </c>
-      <c r="N61">
+      <c r="N65">
         <v>7244</v>
       </c>
-      <c r="O61">
+      <c r="O65">
         <v>24148</v>
       </c>
-      <c r="P61">
+      <c r="P65">
         <v>32372</v>
       </c>
-      <c r="Q61">
+      <c r="Q65">
         <v>24569</v>
       </c>
-      <c r="R61">
+      <c r="R65">
         <v>10277</v>
       </c>
-      <c r="S61">
+      <c r="S65">
         <v>12696</v>
       </c>
-      <c r="T61">
+      <c r="T65">
         <v>25818</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A69">
+        <v>5000</v>
+      </c>
+      <c r="B69">
+        <f>AVERAGE(C69:G69)</f>
+        <v>6256000</v>
+      </c>
+      <c r="C69">
+        <v>15620000</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>15660000</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A70">
+        <v>15000</v>
+      </c>
+      <c r="B70">
+        <f t="shared" ref="B70:B74" si="1">AVERAGE(C70:G70)</f>
+        <v>46871800</v>
+      </c>
+      <c r="C70">
+        <v>46863000</v>
+      </c>
+      <c r="D70">
+        <v>46862000</v>
+      </c>
+      <c r="E70">
+        <v>46869000</v>
+      </c>
+      <c r="F70">
+        <v>46861000</v>
+      </c>
+      <c r="G70">
+        <v>46904000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A71">
+        <v>30000</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="1"/>
+        <v>181206600</v>
+      </c>
+      <c r="C71">
+        <v>171794000</v>
+      </c>
+      <c r="D71">
+        <v>187493000</v>
+      </c>
+      <c r="E71">
+        <v>171833000</v>
+      </c>
+      <c r="F71">
+        <v>187419000</v>
+      </c>
+      <c r="G71">
+        <v>187494000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A72">
+        <v>50000</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="1"/>
+        <v>480430600</v>
+      </c>
+      <c r="C72">
+        <v>472017000</v>
+      </c>
+      <c r="D72">
+        <v>484222000</v>
+      </c>
+      <c r="E72">
+        <v>487410000</v>
+      </c>
+      <c r="F72">
+        <v>474202000</v>
+      </c>
+      <c r="G72">
+        <v>484302000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A73">
+        <v>75000</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="1"/>
+        <v>1077662400</v>
+      </c>
+      <c r="C73">
+        <v>1080389000</v>
+      </c>
+      <c r="D73">
+        <v>1077871000</v>
+      </c>
+      <c r="E73">
+        <v>1065601000</v>
+      </c>
+      <c r="F73">
+        <v>1084037000</v>
+      </c>
+      <c r="G73">
+        <v>1080414000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A74">
+        <v>105000</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="1"/>
+        <v>2179729600</v>
+      </c>
+      <c r="C74">
+        <v>2189571000</v>
+      </c>
+      <c r="D74">
+        <v>2173622000</v>
+      </c>
+      <c r="E74">
+        <v>2171406000</v>
+      </c>
+      <c r="F74">
+        <v>2190373000</v>
+      </c>
+      <c r="G74">
+        <v>2173676000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
+        <v>21</v>
+      </c>
+      <c r="B76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A77">
+        <v>177147</v>
+      </c>
+      <c r="B77">
+        <f>AVERAGE(C77:G77)</f>
+        <v>9609000</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>15603000</v>
+      </c>
+      <c r="E77">
+        <v>15621000</v>
+      </c>
+      <c r="F77">
+        <v>16821000</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A78">
+        <v>531441</v>
+      </c>
+      <c r="B78">
+        <f t="shared" ref="B78:B82" si="2">AVERAGE(C78:G78)</f>
+        <v>31241400</v>
+      </c>
+      <c r="C78">
+        <v>31284000</v>
+      </c>
+      <c r="D78">
+        <v>31241000</v>
+      </c>
+      <c r="E78">
+        <v>31197000</v>
+      </c>
+      <c r="F78">
+        <v>31243000</v>
+      </c>
+      <c r="G78">
+        <v>31242000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A79">
+        <v>1594323</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="2"/>
+        <v>96852200</v>
+      </c>
+      <c r="C79">
+        <v>93735000</v>
+      </c>
+      <c r="D79">
+        <v>93722000</v>
+      </c>
+      <c r="E79">
+        <v>93731000</v>
+      </c>
+      <c r="F79">
+        <v>93726000</v>
+      </c>
+      <c r="G79">
+        <v>109347000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A80">
+        <v>4782969</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="2"/>
+        <v>284821800</v>
+      </c>
+      <c r="C80">
+        <v>312433000</v>
+      </c>
+      <c r="D80">
+        <v>298217000</v>
+      </c>
+      <c r="E80">
+        <v>266714000</v>
+      </c>
+      <c r="F80">
+        <v>281181000</v>
+      </c>
+      <c r="G80">
+        <v>265564000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A81">
+        <v>14348907</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="2"/>
+        <v>809747800</v>
+      </c>
+      <c r="C81">
+        <v>814981000</v>
+      </c>
+      <c r="D81">
+        <v>784478000</v>
+      </c>
+      <c r="E81">
+        <v>799321000</v>
+      </c>
+      <c r="F81">
+        <v>783539000</v>
+      </c>
+      <c r="G81">
+        <v>866420000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A82">
+        <v>43046721</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="2"/>
+        <v>2433408400</v>
+      </c>
+      <c r="C82">
+        <v>2430119000</v>
+      </c>
+      <c r="D82">
+        <v>2427232000</v>
+      </c>
+      <c r="E82">
+        <v>2446111000</v>
+      </c>
+      <c r="F82">
+        <v>2428909000</v>
+      </c>
+      <c r="G82">
+        <v>2434671000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajout tableaux et graphiques dans rapport
</commit_message>
<xml_diff>
--- a/valeurs_expe.xlsx
+++ b/valeurs_expe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SU-ANNESOPHIE\Documents\GitHub\HEIG_ASD1_LABO_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arbroween\Documents\ecole\HEIG-VD\2e_Semestre\ASD1\Laboratoire\Labo1\HEIG_ASD1_LABO_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEAB056-2E11-4C6A-AF01-A4585BC57E47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B775EAF3-DB1A-43AB-A837-DFD225C45B9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{666A6892-ED96-4155-B69D-7B7D26C674DE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{666A6892-ED96-4155-B69D-7B7D26C674DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>Fonction chercherPosition() :</t>
   </si>
@@ -86,9 +86,6 @@
     <t>moyenne temps</t>
   </si>
   <si>
-    <t>nb it</t>
-  </si>
-  <si>
     <t>nb itérations</t>
   </si>
   <si>
@@ -102,6 +99,21 @@
   </si>
   <si>
     <t>(ancien)</t>
+  </si>
+  <si>
+    <t>nb comparaisons</t>
+  </si>
+  <si>
+    <t>nb additions</t>
+  </si>
+  <si>
+    <t>nb d'additions</t>
+  </si>
+  <si>
+    <t>temps moyen</t>
+  </si>
+  <si>
+    <t>théorique</t>
   </si>
 </sst>
 </file>
@@ -199,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -208,6 +220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2634,6 +2647,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CH"/>
+              <a:t>random</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6892,16 +6930,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>180782</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>752282</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>85115</xdr:rowOff>
+      <xdr:rowOff>31775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>180780</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>752280</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>117140</xdr:rowOff>
+      <xdr:rowOff>63800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6928,16 +6966,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>705068</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>24815</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>293588</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>47675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>705070</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>53062</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>293590</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>75922</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6964,16 +7002,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>448649</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>761069</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>53641</xdr:rowOff>
+      <xdr:rowOff>7921</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>448647</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>761067</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>82215</xdr:rowOff>
+      <xdr:rowOff>36495</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7000,16 +7038,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>411165</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>312105</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>131226</xdr:rowOff>
+      <xdr:rowOff>123606</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>411167</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>312107</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>159802</xdr:rowOff>
+      <xdr:rowOff>152182</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7036,14 +7074,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>105104</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>569924</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>161018</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>105105</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>569925</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>17229</xdr:rowOff>
     </xdr:to>
@@ -7072,16 +7110,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>282800</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>534260</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>64079</xdr:rowOff>
+      <xdr:rowOff>109799</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>282801</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>534261</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>117867</xdr:rowOff>
+      <xdr:rowOff>163587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7108,16 +7146,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>274246</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>129693</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>525706</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>38253</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>274247</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>183481</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>525707</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>84421</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7444,16 +7482,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85499602-D119-4872-92A1-2FAD642673CF}">
   <dimension ref="A1:T82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="48" workbookViewId="0">
-      <selection activeCell="M52" sqref="M52"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.46484375" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7462,7 +7500,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -7489,7 +7527,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -7516,7 +7554,7 @@
         <v>3674</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -7543,7 +7581,7 @@
         <v>21555</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -7570,135 +7608,179 @@
         <v>1833</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>6</v>
       </c>
       <c r="C8">
         <v>4032</v>
       </c>
+      <c r="D8">
+        <v>36</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>7</v>
       </c>
       <c r="C9" s="4">
         <v>16256</v>
       </c>
+      <c r="D9">
+        <v>49</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>8</v>
       </c>
       <c r="C10" s="4">
         <v>65280</v>
       </c>
+      <c r="D10">
+        <v>64</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>9</v>
       </c>
       <c r="C11" s="4">
         <v>261632</v>
       </c>
+      <c r="D11">
+        <v>81</v>
+      </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <v>10</v>
       </c>
       <c r="C12" s="4">
         <v>1047552</v>
       </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <v>11</v>
       </c>
       <c r="C13" s="4">
         <v>4192256</v>
       </c>
+      <c r="D13">
+        <v>121</v>
+      </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <v>6</v>
       </c>
       <c r="C16" s="4">
         <v>6</v>
       </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <v>7</v>
       </c>
       <c r="C17" s="4">
         <v>7</v>
       </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <v>8</v>
       </c>
       <c r="C18" s="4">
         <v>8</v>
       </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <v>9</v>
       </c>
       <c r="C19" s="4">
         <v>9</v>
       </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <v>10</v>
       </c>
       <c r="C20" s="4">
         <v>10</v>
       </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <v>11</v>
       </c>
       <c r="C21" s="4">
         <v>11</v>
       </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -7706,141 +7788,189 @@
         <v>8</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <v>11</v>
       </c>
       <c r="C24" s="4">
         <v>177147</v>
       </c>
+      <c r="D24">
+        <v>177147</v>
+      </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <v>12</v>
       </c>
       <c r="C25" s="4">
         <v>531441</v>
       </c>
+      <c r="D25">
+        <v>531441</v>
+      </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <v>13</v>
       </c>
       <c r="C26" s="4">
         <v>1594323</v>
       </c>
+      <c r="D26">
+        <v>1594323</v>
+      </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <v>14</v>
       </c>
       <c r="C27" s="4">
         <v>4782969</v>
       </c>
+      <c r="D27">
+        <v>4782969</v>
+      </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <v>15</v>
       </c>
       <c r="C28" s="4">
         <v>14348907</v>
       </c>
+      <c r="D28">
+        <v>14348907</v>
+      </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <v>16</v>
       </c>
       <c r="C29" s="4">
         <v>43046721</v>
       </c>
+      <c r="D29">
+        <v>43046721</v>
+      </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <v>17</v>
       </c>
       <c r="C30" s="4">
         <v>129140163</v>
       </c>
+      <c r="D30">
+        <v>129140163</v>
+      </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" s="3">
         <v>18</v>
       </c>
       <c r="C31" s="4">
         <v>387420489</v>
       </c>
+      <c r="D31">
+        <v>387420489</v>
+      </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B32" s="3"/>
       <c r="C32" s="4"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>3</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>6561</v>
       </c>
       <c r="C34">
         <v>85293</v>
       </c>
+      <c r="D34">
+        <v>85293</v>
+      </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>19683</v>
       </c>
       <c r="C35">
         <v>295245</v>
       </c>
+      <c r="D35">
+        <v>295245</v>
+      </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>59049</v>
       </c>
       <c r="C36">
         <v>944784</v>
       </c>
+      <c r="D36">
+        <v>944784</v>
+      </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>177147</v>
       </c>
       <c r="C37">
         <v>3188646</v>
       </c>
+      <c r="D37">
+        <v>3188646</v>
+      </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>531441</v>
       </c>
       <c r="C38">
         <v>10628820</v>
       </c>
+      <c r="D38">
+        <v>10628820</v>
+      </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>1594323</v>
       </c>
       <c r="C39">
         <v>33480783</v>
       </c>
+      <c r="D39">
+        <v>33480783</v>
+      </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B40" s="3"/>
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -7851,9 +7981,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B42" s="3">
         <v>10000</v>
@@ -7878,7 +8008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B43" s="3">
         <v>100000</v>
       </c>
@@ -7902,7 +8032,7 @@
         <v>2989000</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B44" s="3">
         <v>1000000</v>
       </c>
@@ -7926,7 +8056,7 @@
         <v>45943000</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B45" s="3">
         <v>10000000</v>
       </c>
@@ -7950,11 +8080,11 @@
         <v>581723000</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B46" s="3"/>
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -7965,9 +8095,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B48" s="3">
         <v>729</v>
@@ -7992,7 +8122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B49" s="3">
         <v>2187</v>
       </c>
@@ -8016,7 +8146,7 @@
         <v>2119000</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B50" s="3">
         <v>6561</v>
       </c>
@@ -8040,7 +8170,7 @@
         <v>6604000</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B51" s="3">
         <v>19683</v>
       </c>
@@ -8064,7 +8194,7 @@
         <v>75342000</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B52" s="5">
         <v>59049</v>
       </c>
@@ -8088,12 +8218,12 @@
         <v>683646000</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>13</v>
       </c>
@@ -8104,7 +8234,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2187</v>
       </c>
@@ -8167,7 +8297,7 @@
         <v>2187</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>6561</v>
       </c>
@@ -8230,7 +8360,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>19683</v>
       </c>
@@ -8293,7 +8423,7 @@
         <v>16387</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>59049</v>
       </c>
@@ -8356,7 +8486,7 @@
         <v>51266</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>177147</v>
       </c>
@@ -8419,7 +8549,7 @@
         <v>40161</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>531441</v>
       </c>
@@ -8482,7 +8612,7 @@
         <v>22801</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>1594323</v>
       </c>
@@ -8545,7 +8675,7 @@
         <v>104805</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>4782969</v>
       </c>
@@ -8608,7 +8738,7 @@
         <v>25646</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>14348907</v>
       </c>
@@ -8671,7 +8801,7 @@
         <v>30933</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>43046721</v>
       </c>
@@ -8734,15 +8864,15 @@
         <v>25818</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B68" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>5000</v>
       </c>
@@ -8766,7 +8896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>15000</v>
       </c>
@@ -8790,7 +8920,7 @@
         <v>46904000</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>30000</v>
       </c>
@@ -8814,7 +8944,7 @@
         <v>187494000</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>50000</v>
       </c>
@@ -8838,7 +8968,7 @@
         <v>484302000</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>75000</v>
       </c>
@@ -8862,7 +8992,7 @@
         <v>1080414000</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>105000</v>
       </c>
@@ -8886,15 +9016,15 @@
         <v>2173676000</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B76" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>177147</v>
       </c>
@@ -8918,7 +9048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>531441</v>
       </c>
@@ -8942,7 +9072,7 @@
         <v>31242000</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>1594323</v>
       </c>
@@ -8966,7 +9096,7 @@
         <v>109347000</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>4782969</v>
       </c>
@@ -8990,7 +9120,7 @@
         <v>265564000</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>14348907</v>
       </c>
@@ -9014,7 +9144,7 @@
         <v>866420000</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>43046721</v>
       </c>

</xml_diff>

<commit_message>
correction trier et chercherSiContient
</commit_message>
<xml_diff>
--- a/valeurs_expe.xlsx
+++ b/valeurs_expe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SU-ANNESOPHIE\Documents\GitHub\HEIG_ASD1_LABO_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E701EAF-354F-4D84-BDBD-C666046BBDE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3460DDC0-E290-4046-A060-644511441F4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{666A6892-ED96-4155-B69D-7B7D26C674DE}"/>
   </bookViews>
@@ -1160,7 +1160,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="log"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -1207,22 +1207,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>2048</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1275,8 +1275,9 @@
       <c:valAx>
         <c:axId val="465551192"/>
         <c:scaling>
+          <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:min val="5"/>
+          <c:min val="64"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1294,6 +1295,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CH"/>
+                  <a:t>taille tableau</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1357,6 +1413,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CH"/>
+                  <a:t>nb iteration</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1560,7 +1671,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="exp"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -1607,22 +1718,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>2048</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1675,8 +1786,10 @@
       <c:valAx>
         <c:axId val="454866968"/>
         <c:scaling>
+          <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:min val="6"/>
+          <c:max val="4096"/>
+          <c:min val="32"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1694,6 +1807,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CH"/>
+                  <a:t>taille tableau</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1758,6 +1926,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CH"/>
+                  <a:t>nb iterations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -7264,15 +7487,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>761069</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>7921</xdr:rowOff>
+      <xdr:colOff>122894</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>22209</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>761067</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>36495</xdr:rowOff>
+      <xdr:colOff>122892</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>50783</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7743,8 +7966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85499602-D119-4872-92A1-2FAD642673CF}">
   <dimension ref="A1:T79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K23" zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N43" sqref="N43"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7889,7 +8112,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B8" s="3">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="C8">
         <v>4032</v>
@@ -7900,7 +8123,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B9" s="3">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="C9" s="4">
         <v>16256</v>
@@ -7911,7 +8134,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B10" s="3">
-        <v>8</v>
+        <v>256</v>
       </c>
       <c r="C10" s="4">
         <v>65280</v>
@@ -7922,7 +8145,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B11" s="3">
-        <v>9</v>
+        <v>512</v>
       </c>
       <c r="C11" s="4">
         <v>261632</v>
@@ -7933,7 +8156,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B12" s="3">
-        <v>10</v>
+        <v>1024</v>
       </c>
       <c r="C12" s="4">
         <v>1047552</v>
@@ -7944,7 +8167,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B13" s="3">
-        <v>11</v>
+        <v>2048</v>
       </c>
       <c r="C13" s="4">
         <v>4192256</v>
@@ -7973,7 +8196,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B16" s="3">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="C16" s="4">
         <v>6</v>
@@ -7984,7 +8207,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B17" s="3">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="C17" s="4">
         <v>7</v>
@@ -7995,7 +8218,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B18" s="3">
-        <v>8</v>
+        <v>256</v>
       </c>
       <c r="C18" s="4">
         <v>8</v>
@@ -8006,7 +8229,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B19" s="3">
-        <v>9</v>
+        <v>512</v>
       </c>
       <c r="C19" s="4">
         <v>9</v>
@@ -8017,7 +8240,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B20" s="3">
-        <v>10</v>
+        <v>1024</v>
       </c>
       <c r="C20" s="4">
         <v>10</v>
@@ -8028,7 +8251,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B21" s="3">
-        <v>11</v>
+        <v>2048</v>
       </c>
       <c r="C21" s="4">
         <v>11</v>

</xml_diff>